<commit_message>
add some graphs to Graph folder, add some SQL files
</commit_message>
<xml_diff>
--- a/minuteSummary.xlsx
+++ b/minuteSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lynda.com\Data Analytics\Google Analytics Certificate\8-Capstone Project\BellaBeat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7B7077-97FC-4B58-BDBA-6BAC3B3A0A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8540BB98-751A-42AC-A744-85D829359B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="minuteNumericSummary" sheetId="1" r:id="rId1"/>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC539F1-C337-4101-BB2A-66BD75DE37BB}">
   <dimension ref="A1:C1441"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -12689,7 +12689,7 @@
   <dimension ref="A1:M1441"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>